<commit_message>
GETs and POSTs for registration and profiles.
</commit_message>
<xml_diff>
--- a/User_Interface/test/user_interface_testplan.xlsx
+++ b/User_Interface/test/user_interface_testplan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26819"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="-460" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="44">
   <si>
     <t>Test #</t>
   </si>
@@ -130,13 +130,34 @@
   </si>
   <si>
     <t>There is an error in the web configuration that does not allows me to render data from the JSON</t>
+  </si>
+  <si>
+    <t>Pass Condition</t>
+  </si>
+  <si>
+    <t>Fail Condition</t>
+  </si>
+  <si>
+    <t>All required fields completed</t>
+  </si>
+  <si>
+    <t>Missing required fields</t>
+  </si>
+  <si>
+    <t>Deletion success</t>
+  </si>
+  <si>
+    <t>No module found</t>
+  </si>
+  <si>
+    <t>No account found</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -181,6 +202,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -215,14 +243,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
@@ -248,11 +288,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="17">
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -583,23 +638,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="20.6640625" customWidth="1"/>
     <col min="3" max="3" width="75.6640625" customWidth="1"/>
-    <col min="4" max="4" width="32.6640625" customWidth="1"/>
-    <col min="5" max="5" width="20" customWidth="1"/>
-    <col min="6" max="6" width="34.5" customWidth="1"/>
-    <col min="7" max="7" width="30" customWidth="1"/>
+    <col min="4" max="6" width="32.6640625" customWidth="1"/>
+    <col min="7" max="7" width="20" customWidth="1"/>
+    <col min="8" max="8" width="34.5" customWidth="1"/>
+    <col min="9" max="9" width="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="5" customFormat="1" ht="18">
+    <row r="1" spans="1:9" s="5" customFormat="1" ht="18">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -613,16 +668,22 @@
         <v>17</v>
       </c>
       <c r="E1" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="30">
+    <row r="2" spans="1:9" ht="30">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -635,15 +696,21 @@
       <c r="D2" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="6">
+      <c r="H2" s="6">
         <v>0.1</v>
       </c>
-      <c r="G2" s="10"/>
-    </row>
-    <row r="3" spans="1:7" ht="30">
+      <c r="I2" s="10"/>
+    </row>
+    <row r="3" spans="1:9" ht="30">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -656,15 +723,21 @@
       <c r="D3" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="6">
+      <c r="H3" s="6">
         <v>0.2</v>
       </c>
-      <c r="G3" s="10"/>
-    </row>
-    <row r="4" spans="1:7" ht="30">
+      <c r="I3" s="10"/>
+    </row>
+    <row r="4" spans="1:9" ht="30">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -677,15 +750,21 @@
       <c r="D4" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="6">
+      <c r="H4" s="6">
         <v>0.3</v>
       </c>
-      <c r="G4" s="10"/>
-    </row>
-    <row r="5" spans="1:7" ht="45">
+      <c r="I4" s="10"/>
+    </row>
+    <row r="5" spans="1:9" ht="45">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -698,17 +777,23 @@
       <c r="D5" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="6">
+      <c r="H5" s="6">
         <v>0.05</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="I5" s="9" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="45">
+    <row r="6" spans="1:9" ht="45">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -721,17 +806,23 @@
       <c r="D6" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="6">
+      <c r="H6" s="6">
         <v>0.05</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="I6" s="9" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="45">
+    <row r="7" spans="1:9" ht="45">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -744,17 +835,23 @@
       <c r="D7" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="6">
+      <c r="H7" s="6">
         <v>0.05</v>
       </c>
-      <c r="G7" s="9" t="s">
+      <c r="I7" s="9" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="45">
+    <row r="8" spans="1:9" ht="45">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -767,17 +864,23 @@
       <c r="D8" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="G8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F8" s="6">
+      <c r="H8" s="6">
         <v>0.1</v>
       </c>
-      <c r="G8" s="9" t="s">
+      <c r="I8" s="9" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="45">
+    <row r="9" spans="1:9" ht="45">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -790,17 +893,23 @@
       <c r="D9" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="G9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F9" s="6">
+      <c r="H9" s="6">
         <v>0.05</v>
       </c>
-      <c r="G9" s="9" t="s">
+      <c r="I9" s="9" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="45">
+    <row r="10" spans="1:9" ht="45">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -813,27 +922,33 @@
       <c r="D10" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="G10" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="6">
+      <c r="H10" s="6">
         <v>0.05</v>
       </c>
-      <c r="G10" s="9" t="s">
+      <c r="I10" s="9" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
-      <c r="E11" t="s">
+    <row r="11" spans="1:9">
+      <c r="G11" t="s">
         <v>35</v>
       </c>
-      <c r="F11" s="8">
+      <c r="H11" s="8">
         <v>1</v>
       </c>
-      <c r="G11" s="10"/>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="F12" s="7"/>
+      <c r="I11" s="10"/>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="H12" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>